<commit_message>
update context menu logplot
</commit_message>
<xml_diff>
--- a/Wi-LogPlot.xlsx
+++ b/Wi-LogPlot.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TooNies1810/Documents/lab/ribon-angular/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LogPlotTab" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -455,10 +459,10 @@
     <t>ScaleDropdown</t>
   </si>
   <si>
-    <t>properties_16x16</t>
-  </si>
-  <si>
     <t>arrow_right_16x16</t>
+  </si>
+  <si>
+    <t>track_properties_16x16</t>
   </si>
 </sst>
 </file>
@@ -813,7 +817,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -823,21 +827,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="5"/>
-    <col min="2" max="2" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.875" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
     <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.875" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -912,11 +916,11 @@
         <v>Button</v>
       </c>
       <c r="E3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F3" t="str">
         <f>SUBSTITUTE(E3,"_","-")</f>
-        <v>properties-16x16</v>
+        <v>track-properties-16x16</v>
       </c>
       <c r="J3" t="s">
         <v>13</v>
@@ -1024,7 +1028,7 @@
         <v>Button</v>
       </c>
       <c r="E7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -1948,7 +1952,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>7.2</v>
       </c>
@@ -1970,7 +1974,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
         <v>7.3</v>
       </c>
@@ -2006,7 +2010,7 @@
       <selection sqref="A1:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>